<commit_message>
upgraded to selenium 4.x
</commit_message>
<xml_diff>
--- a/resources/reports/ExcelReport.xlsx
+++ b/resources/reports/ExcelReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="48">
   <si>
     <t>OPEN BOWSER</t>
   </si>
@@ -29,91 +29,143 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>6:11:48 PM</t>
-  </si>
-  <si>
-    <t>Lanuch Browser--chrome</t>
-  </si>
-  <si>
-    <t>6:11:50 PM</t>
-  </si>
-  <si>
-    <t>Enter URL--https://demo.nopcommerce.com/</t>
-  </si>
-  <si>
-    <t>6:11:51 PM</t>
-  </si>
-  <si>
-    <t>Verify nopcommerce logo : Element is Present</t>
-  </si>
-  <si>
-    <t>Info</t>
+    <t>4:26:13 PM</t>
+  </si>
+  <si>
+    <t>Lanuch browser--chrome</t>
+  </si>
+  <si>
+    <t>4:26:15 PM</t>
+  </si>
+  <si>
+    <t>Enter URL--https://www.ratnaglobaltech.com/</t>
+  </si>
+  <si>
+    <t>Verify Logo is displayed or not : Element is Present</t>
+  </si>
+  <si>
+    <t>verify Email id--Actual:contact@ratnaglobaltech.com--Expected:contact@ratnaglobaltech.com</t>
+  </si>
+  <si>
+    <t>Close browser</t>
+  </si>
+  <si>
+    <t>4:26:17 PM</t>
+  </si>
+  <si>
+    <t>4:26:22 PM</t>
+  </si>
+  <si>
+    <t>Enter URL--https://www.amazon.in/</t>
+  </si>
+  <si>
+    <t>4:26:27 PM</t>
+  </si>
+  <si>
+    <t>Mousehover on Accounts and Lists : Mouse hovered on element</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Click on sign in is Failed</t>
+  </si>
+  <si>
+    <t>org.openqa.selenium.ElementNotInteractableException: element not interactable
+  (Session info: chrome=115.0.5790.110)
+Build info: version: '4.10.0', revision: 'c14d967899'
+System info: os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Command: [0552697881153704d0ce7eb3e0650048, clickElement {id=08D0257B693C2F4D2748282934BFE048_element_26}]
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 115.0.5790.110, chrome: {chromedriverVersion: 114.0.5735.90 (386bc09e8f4f..., userDataDir: C:\Users\ROOPAV~1\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52677}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:52677/devtoo..., se:cdpVersion: 115.0.5790.110, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Element: [[ChromeDriver: chrome on windows (0552697881153704d0ce7eb3e0650048)] -&gt; xpath: //*[@id="nav-flyout-ya-signin"]/a/span]
+Session ID: 0552697881153704d0ce7eb3e0650048</t>
+  </si>
+  <si>
+    <t>4:26:28 PM</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Take sElement screenshot of Logo :Element Screenshot captured</t>
-  </si>
-  <si>
-    <t>6:11:53 PM</t>
-  </si>
-  <si>
-    <t>Click on Register : Element clicked</t>
-  </si>
-  <si>
-    <t>Select Gender radio button : Element clicked</t>
-  </si>
-  <si>
-    <t>Enter First Name:Sai Ram</t>
-  </si>
-  <si>
-    <t>Enter Last Name:Pendem</t>
-  </si>
-  <si>
-    <t>6:11:54 PM</t>
-  </si>
-  <si>
-    <t>Choose Date of birth (Date):Selected Value By SELECTBYVALUE is 6</t>
-  </si>
-  <si>
-    <t>Choose Date of birth (Month):Selected Value By SELECTBYVISIBILETEXT is August</t>
-  </si>
-  <si>
-    <t>6:11:55 PM</t>
-  </si>
-  <si>
-    <t>Choose Date of birth (Year):Selected Value By SELECTBYVALUE is 2000</t>
-  </si>
-  <si>
-    <t>Enter Email address:sairamprince019@gmail.com</t>
-  </si>
-  <si>
-    <t>Enter company name:Ratna Global Technologies</t>
-  </si>
-  <si>
-    <t>6:11:56 PM</t>
-  </si>
-  <si>
-    <t>Enter password:Sairam@123</t>
-  </si>
-  <si>
-    <t>Enter Confirm passowrd:Sairam@123</t>
-  </si>
-  <si>
-    <t>6:11:58 PM</t>
-  </si>
-  <si>
-    <t>Click on Register button : Element clicked</t>
-  </si>
-  <si>
-    <t>Take screenshot of registration completed message : Screenshot captured</t>
-  </si>
-  <si>
-    <t>6:11:59 PM</t>
-  </si>
-  <si>
-    <t>Verify Registration completed message--Actual:Your registration completed--Expected:Your registration completed</t>
+    <t>Click on sign in - Test case failed base64 img</t>
+  </si>
+  <si>
+    <t>Enter Eamil or phone number is Failed</t>
+  </si>
+  <si>
+    <t>org.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"css selector","selector":"#ap_email"}
+  (Session info: chrome=115.0.5790.110)
+For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Build info: version: '4.10.0', revision: 'c14d967899'
+System info: os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Command: [0552697881153704d0ce7eb3e0650048, findElement {using=id, value=ap_email}]
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 115.0.5790.110, chrome: {chromedriverVersion: 114.0.5735.90 (386bc09e8f4f..., userDataDir: C:\Users\ROOPAV~1\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52677}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:52677/devtoo..., se:cdpVersion: 115.0.5790.110, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 0552697881153704d0ce7eb3e0650048</t>
+  </si>
+  <si>
+    <t>4:26:29 PM</t>
+  </si>
+  <si>
+    <t>Enter Eamil or phone number - Test case failed base64 img</t>
+  </si>
+  <si>
+    <t>Click on continue button is Failed</t>
+  </si>
+  <si>
+    <t>org.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"//*[@id="continue"]"}
+  (Session info: chrome=115.0.5790.110)
+For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Build info: version: '4.10.0', revision: 'c14d967899'
+System info: os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Command: [0552697881153704d0ce7eb3e0650048, findElement {using=xpath, value=//*[@id="continue"]}]
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 115.0.5790.110, chrome: {chromedriverVersion: 114.0.5735.90 (386bc09e8f4f..., userDataDir: C:\Users\ROOPAV~1\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52677}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:52677/devtoo..., se:cdpVersion: 115.0.5790.110, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 0552697881153704d0ce7eb3e0650048</t>
+  </si>
+  <si>
+    <t>4:26:30 PM</t>
+  </si>
+  <si>
+    <t>Click on continue button - Test case failed base64 img</t>
+  </si>
+  <si>
+    <t>Enter password is Failed</t>
+  </si>
+  <si>
+    <t>org.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"css selector","selector":"*[name='password']"}
+  (Session info: chrome=115.0.5790.110)
+For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Build info: version: '4.10.0', revision: 'c14d967899'
+System info: os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Command: [0552697881153704d0ce7eb3e0650048, findElement {using=name, value=password}]
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 115.0.5790.110, chrome: {chromedriverVersion: 114.0.5735.90 (386bc09e8f4f..., userDataDir: C:\Users\ROOPAV~1\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52677}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:52677/devtoo..., se:cdpVersion: 115.0.5790.110, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 0552697881153704d0ce7eb3e0650048</t>
+  </si>
+  <si>
+    <t>Enter password - Test case failed base64 img</t>
+  </si>
+  <si>
+    <t>Click on sign in button is Failed</t>
+  </si>
+  <si>
+    <t>org.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"//*[@id="signInSubmit"]"}
+  (Session info: chrome=115.0.5790.110)
+For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Build info: version: '4.10.0', revision: 'c14d967899'
+System info: os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Command: [0552697881153704d0ce7eb3e0650048, findElement {using=xpath, value=//*[@id="signInSubmit"]}]
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 115.0.5790.110, chrome: {chromedriverVersion: 114.0.5735.90 (386bc09e8f4f..., userDataDir: C:\Users\ROOPAV~1\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52677}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:52677/devtoo..., se:cdpVersion: 115.0.5790.110, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 0552697881153704d0ce7eb3e0650048</t>
+  </si>
+  <si>
+    <t>4:26:31 PM</t>
+  </si>
+  <si>
+    <t>Click on sign in button - Test case failed base64 img</t>
   </si>
   <si>
     <t>username</t>
@@ -201,7 +253,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -246,21 +298,21 @@
         <v>4</v>
       </c>
       <c r="B5" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s" s="0">
         <v>9</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -268,32 +320,22 @@
         <v>4</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>15</v>
-      </c>
-    </row>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8"/>
     <row r="9">
       <c r="A9" t="s" s="0">
         <v>4</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10">
@@ -301,10 +343,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s" s="0">
         <v>14</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>17</v>
       </c>
     </row>
     <row r="11">
@@ -312,10 +354,10 @@
         <v>4</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12">
@@ -323,161 +365,282 @@
         <v>4</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s" s="0">
         <v>22</v>
-      </c>
-      <c r="C16" t="s" s="0">
-        <v>25</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>35</v>
+        <v>29</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>30</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>31</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>39</v>
+        <v>29</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>32</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>41</v>
+        <v>29</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>21</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="C32" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="C33" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34"/>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="B28" t="s" s="0">
+      <c r="B37" t="s" s="0">
         <v>43</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>